<commit_message>
update metadata and running round4 imaging
</commit_message>
<xml_diff>
--- a/paramaters/MouseCity_round2.xlsx
+++ b/paramaters/MouseCity_round2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\DELTA_iDISCO\paramaters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54810310-69A0-424F-8EEB-164C8DAF6358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2638C5B1-5789-40E2-9F37-517E94733682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3468" windowWidth="19464" windowHeight="11232" activeTab="2" xr2:uid="{B7DD41B0-567A-4A82-BB1D-646583CE9931}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="16044" windowHeight="10944" activeTab="2" xr2:uid="{B7DD41B0-567A-4A82-BB1D-646583CE9931}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre" sheetId="1" r:id="rId1"/>
@@ -1331,11 +1331,12 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>